<commit_message>
refactor of Master class. check_project_information function included. check_baselines function included as option
</commit_message>
<xml_diff>
--- a/tests/resources/test_project_group_id_no.xlsx
+++ b/tests/resources/test_project_group_id_no.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="112">
   <si>
     <t xml:space="preserve">Projects</t>
   </si>
@@ -94,15 +94,6 @@
   </si>
   <si>
     <t xml:space="preserve">F9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Live </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Live</t>
   </si>
   <si>
     <t xml:space="preserve">Q1 2021</t>
@@ -577,7 +568,7 @@
   <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -679,24 +670,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="C5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C6" s="2"/>
@@ -833,9 +807,7 @@
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C50" s="2"/>
     </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C51" s="2"/>
-    </row>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -847,7 +819,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <conditionalFormatting sqref="C1:C51">
+  <conditionalFormatting sqref="C1:C50">
     <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="md" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("md",C1)))</formula>
     </cfRule>
@@ -889,523 +861,523 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1413,7 +1385,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>11</v>
@@ -1431,7 +1403,7 @@
         <v>11</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>11</v>
@@ -1458,7 +1430,7 @@
         <v>11</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1466,7 +1438,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>11</v>
@@ -1490,28 +1462,28 @@
         <v>11</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1519,7 +1491,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>11</v>
@@ -1537,7 +1509,7 @@
         <v>11</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>11</v>
@@ -1558,13 +1530,13 @@
         <v>11</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1572,7 +1544,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>10</v>
@@ -1599,25 +1571,25 @@
         <v>10</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1625,7 +1597,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>10</v>
@@ -1643,7 +1615,7 @@
         <v>10</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>10</v>
@@ -1675,55 +1647,55 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1731,7 +1703,7 @@
         <v>11</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>11</v>
@@ -1749,7 +1721,7 @@
         <v>11</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>11</v>
@@ -1784,7 +1756,7 @@
         <v>10</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>10</v>
@@ -1823,13 +1795,13 @@
         <v>11</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1837,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>10</v>
@@ -1870,19 +1842,19 @@
         <v>10</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="N19" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="O19" s="3" t="s">
         <v>10</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1890,7 +1862,7 @@
         <v>10</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>10</v>
@@ -1923,19 +1895,19 @@
         <v>10</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="O20" s="3" t="s">
         <v>10</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1943,7 +1915,7 @@
         <v>10</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>10</v>
@@ -1976,72 +1948,72 @@
         <v>10</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="N21" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="O21" s="3" t="s">
         <v>10</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2049,7 +2021,7 @@
         <v>11</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>11</v>
@@ -2067,7 +2039,7 @@
         <v>11</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>11</v>
@@ -2099,108 +2071,108 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="Q24" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="Q25" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2208,7 +2180,7 @@
         <v>11</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>11</v>
@@ -2226,7 +2198,7 @@
         <v>11</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>11</v>
@@ -2261,7 +2233,7 @@
         <v>11</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>11</v>
@@ -2273,40 +2245,40 @@
         <v>11</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Q27" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2314,7 +2286,7 @@
         <v>11</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>11</v>
@@ -2326,40 +2298,40 @@
         <v>11</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O28" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2367,7 +2339,7 @@
         <v>10</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>10</v>
@@ -2385,34 +2357,34 @@
         <v>10</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O29" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Q29" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2420,7 +2392,7 @@
         <v>11</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>11</v>
@@ -2438,7 +2410,7 @@
         <v>11</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I30" s="2" t="s">
         <v>11</v>
@@ -2473,7 +2445,7 @@
         <v>11</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>11</v>
@@ -2491,7 +2463,7 @@
         <v>11</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>11</v>
@@ -2526,7 +2498,7 @@
         <v>11</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>11</v>
@@ -2544,7 +2516,7 @@
         <v>11</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>11</v>
@@ -2565,13 +2537,13 @@
         <v>11</v>
       </c>
       <c r="O32" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="Q32" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2579,7 +2551,7 @@
         <v>11</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>11</v>
@@ -2591,40 +2563,40 @@
         <v>11</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O33" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Q33" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2632,7 +2604,7 @@
         <v>11</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>11</v>
@@ -2665,83 +2637,83 @@
         <v>11</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="N34" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O34" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Q34" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="O35" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="Q35" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>10</v>
@@ -2756,7 +2728,7 @@
         <v>10</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I36" s="2" t="s">
         <v>10</v>
@@ -2771,178 +2743,178 @@
         <v>10</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="N36" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="O36" s="3" t="s">
         <v>10</v>
       </c>
       <c r="P36" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="Q36" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="N37" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O37" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="P37" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Q37" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="N38" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O38" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Q38" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="P39" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Q39" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2950,13 +2922,13 @@
         <v>11</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>11</v>
@@ -3003,16 +2975,16 @@
         <v>11</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>11</v>
@@ -3056,16 +3028,16 @@
         <v>11</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>11</v>
@@ -3074,7 +3046,7 @@
         <v>11</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I42" s="2" t="s">
         <v>11</v>
@@ -3109,19 +3081,19 @@
         <v>11</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>11</v>
@@ -3162,19 +3134,19 @@
         <v>11</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>11</v>
@@ -3215,22 +3187,22 @@
         <v>11</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H45" s="2" t="s">
         <v>11</v>
@@ -3251,69 +3223,69 @@
         <v>11</v>
       </c>
       <c r="N45" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O45" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="P45" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Q45" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="M46" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="N46" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="O46" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="P46" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="Q46" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3321,25 +3293,25 @@
         <v>11</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I47" s="2" t="s">
         <v>11</v>
@@ -3374,28 +3346,28 @@
         <v>11</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J48" s="2" t="s">
         <v>11</v>
@@ -3407,178 +3379,178 @@
         <v>11</v>
       </c>
       <c r="M48" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="N48" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O48" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="P48" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Q48" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="M49" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="N49" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O49" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="P49" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Q49" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L50" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="M50" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="N50" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O50" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="P50" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Q50" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L51" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M51" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="N51" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="O51" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="P51" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="Q51" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3586,40 +3558,40 @@
         <v>11</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L52" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M52" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="N52" s="2" t="s">
         <v>11</v>
@@ -3636,161 +3608,161 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L53" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M53" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="N53" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="O53" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="P53" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="Q53" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L54" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M54" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="N54" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="O54" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="P54" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="Q54" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L55" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M55" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="N55" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="O55" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="P55" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="Q55" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3798,40 +3770,40 @@
         <v>11</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L56" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M56" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="N56" s="2" t="s">
         <v>11</v>
@@ -3851,43 +3823,43 @@
         <v>11</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L57" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M57" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="N57" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O57" s="2" t="s">
         <v>11</v>
@@ -3901,161 +3873,161 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L58" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M58" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="N58" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O58" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="P58" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q58" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M59" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="N59" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O59" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="P59" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="Q59" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L60" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M60" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="N60" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O60" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="P60" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Q60" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4063,49 +4035,49 @@
         <v>11</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L61" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M61" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="N61" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O61" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="P61" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Q61" s="1" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
get benefits totals added to BenefitsData class. updates to test master files. tests passing
</commit_message>
<xml_diff>
--- a/tests/resources/test_project_group_id_no.xlsx
+++ b/tests/resources/test_project_group_id_no.xlsx
@@ -920,12 +920,12 @@
           <t>18-19 RDEL Forecast one off new costs</t>
         </is>
       </c>
-      <c r="C23" s="6" t="n"/>
-      <c r="D23" s="6" t="n">
-        <v>0</v>
-      </c>
+      <c r="C23" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" s="6" t="n"/>
       <c r="E23" s="6" t="n">
-        <v>37.88</v>
+        <v>1.08</v>
       </c>
       <c r="F23" s="6" t="n">
         <v>0</v>
@@ -940,11 +940,13 @@
           <t>18-19 RDEL Forecast recurring new costs</t>
         </is>
       </c>
-      <c r="C24" s="6" t="n"/>
-      <c r="D24" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E24" s="6" t="n"/>
+      <c r="C24" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" s="6" t="n"/>
+      <c r="E24" s="6" t="n">
+        <v>0</v>
+      </c>
       <c r="F24" s="6" t="n">
         <v>0</v>
       </c>
@@ -958,10 +960,10 @@
           <t>18-19 RDEL Forecast recurring old costs</t>
         </is>
       </c>
-      <c r="C25" s="6" t="n"/>
-      <c r="D25" s="6" t="n">
-        <v>0</v>
-      </c>
+      <c r="C25" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" s="6" t="n"/>
       <c r="E25" s="6" t="n">
         <v>0</v>
       </c>
@@ -1004,7 +1006,7 @@
         <v>0</v>
       </c>
       <c r="E27" s="6" t="n">
-        <v>37.88</v>
+        <v>1.08</v>
       </c>
       <c r="F27" s="6" t="n">
         <v>0</v>
@@ -1039,16 +1041,16 @@
         </is>
       </c>
       <c r="C29" s="6" t="n">
-        <v>470</v>
+        <v>447.8</v>
       </c>
       <c r="D29" s="6" t="n">
         <v>0</v>
       </c>
       <c r="E29" s="6" t="n">
-        <v>25</v>
+        <v>14.25</v>
       </c>
       <c r="F29" s="6" t="n">
-        <v>61.9</v>
+        <v>78.40000000000001</v>
       </c>
       <c r="G29" s="6" t="n">
         <v>0</v>
@@ -1063,10 +1065,10 @@
       <c r="C30" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="D30" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E30" s="6" t="n"/>
+      <c r="D30" s="6" t="n"/>
+      <c r="E30" s="6" t="n">
+        <v>0</v>
+      </c>
       <c r="F30" s="6" t="n">
         <v>0</v>
       </c>
@@ -1083,9 +1085,7 @@
       <c r="C31" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="D31" s="6" t="n">
-        <v>0</v>
-      </c>
+      <c r="D31" s="6" t="n"/>
       <c r="E31" s="6" t="n">
         <v>0</v>
       </c>
@@ -1102,16 +1102,20 @@
           <t>18-19 Forecast Non-Gov</t>
         </is>
       </c>
-      <c r="C32" s="6" t="n"/>
+      <c r="C32" s="6" t="n">
+        <v>0</v>
+      </c>
       <c r="D32" s="6" t="n">
-        <v>66.09999999999999</v>
+        <v>3.4</v>
       </c>
       <c r="E32" s="6" t="n">
         <v>96</v>
       </c>
-      <c r="F32" s="6" t="n"/>
+      <c r="F32" s="6" t="n">
+        <v>0</v>
+      </c>
       <c r="G32" s="6" t="n">
-        <v>71.09999999999999</v>
+        <v>99.90000000000001</v>
       </c>
     </row>
     <row r="33" ht="13.8" customFormat="1" customHeight="1" s="6">
@@ -1139,9 +1143,15 @@
           <t>18-19 Forecast - Income both Revenue and Capital</t>
         </is>
       </c>
-      <c r="C34" s="6" t="n"/>
-      <c r="E34" s="6" t="n"/>
-      <c r="F34" s="6" t="n"/>
+      <c r="C34" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" s="6" t="n">
+        <v>0</v>
+      </c>
       <c r="G34" s="6" t="n">
         <v>0</v>
       </c>
@@ -1155,12 +1165,12 @@
       <c r="B35" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="C35" s="6" t="n"/>
-      <c r="D35" s="6" t="n">
-        <v>0</v>
-      </c>
+      <c r="C35" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" s="6" t="n"/>
       <c r="E35" s="6" t="n">
-        <v>34.49</v>
+        <v>2</v>
       </c>
       <c r="F35" s="6" t="n">
         <v>0</v>
@@ -1178,11 +1188,13 @@
       <c r="B36" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="C36" s="6" t="n"/>
-      <c r="D36" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E36" s="6" t="n"/>
+      <c r="C36" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" s="6" t="n"/>
+      <c r="E36" s="6" t="n">
+        <v>0</v>
+      </c>
       <c r="F36" s="6" t="n">
         <v>0</v>
       </c>
@@ -1199,10 +1211,10 @@
       <c r="B37" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="C37" s="6" t="n"/>
-      <c r="D37" s="6" t="n">
-        <v>0</v>
-      </c>
+      <c r="C37" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" s="6" t="n"/>
       <c r="E37" s="6" t="n">
         <v>0</v>
       </c>
@@ -1252,7 +1264,7 @@
         <v>0</v>
       </c>
       <c r="E39" s="6" t="n">
-        <v>34.49</v>
+        <v>2</v>
       </c>
       <c r="F39" s="6" t="n">
         <v>0</v>
@@ -1294,7 +1306,7 @@
         <v>0</v>
       </c>
       <c r="C41" s="6" t="n">
-        <v>243.9</v>
+        <v>320.9</v>
       </c>
       <c r="D41" s="6" t="n">
         <v>0</v>
@@ -1303,7 +1315,7 @@
         <v>0</v>
       </c>
       <c r="F41" s="6" t="n">
-        <v>64.3</v>
+        <v>165</v>
       </c>
       <c r="G41" s="6" t="n">
         <v>0</v>
@@ -1321,9 +1333,7 @@
       <c r="C42" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="D42" s="6" t="n">
-        <v>0</v>
-      </c>
+      <c r="D42" s="6" t="n"/>
       <c r="E42" s="6" t="n">
         <v>0</v>
       </c>
@@ -1346,9 +1356,7 @@
       <c r="C43" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="D43" s="6" t="n">
-        <v>0</v>
-      </c>
+      <c r="D43" s="6" t="n"/>
       <c r="E43" s="6" t="n">
         <v>0</v>
       </c>
@@ -1368,16 +1376,20 @@
       <c r="B44" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="C44" s="6" t="n"/>
+      <c r="C44" s="6" t="n">
+        <v>0</v>
+      </c>
       <c r="D44" s="6" t="n">
-        <v>102.8</v>
-      </c>
-      <c r="E44" s="6" t="n"/>
+        <v>22.6</v>
+      </c>
+      <c r="E44" s="6" t="n">
+        <v>0</v>
+      </c>
       <c r="F44" s="6" t="n">
         <v>0</v>
       </c>
       <c r="G44" s="6" t="n">
-        <v>30.7</v>
+        <v>11.7</v>
       </c>
     </row>
     <row r="45" ht="13.8" customHeight="1" s="7">
@@ -1414,10 +1426,16 @@
       <c r="B46" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="C46" s="6" t="n"/>
+      <c r="C46" s="6" t="n">
+        <v>0</v>
+      </c>
       <c r="D46" s="6" t="n"/>
-      <c r="E46" s="6" t="n"/>
-      <c r="F46" s="6" t="n"/>
+      <c r="E46" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" s="6" t="n">
+        <v>0</v>
+      </c>
       <c r="G46" s="6" t="n">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
removal of project specific code. Further abstracting achieved via string_conversion! all tests passing
</commit_message>
<xml_diff>
--- a/tests/resources/test_project_group_id_no.xlsx
+++ b/tests/resources/test_project_group_id_no.xlsx
@@ -451,7 +451,7 @@
   <dimension ref="A1:H71"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G46" activeCellId="0" sqref="B5:G46"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="0" outlineLevelRow="0"/>
@@ -610,835 +610,148 @@
       </c>
     </row>
     <row r="5" ht="13.8" customHeight="1" s="7">
-      <c r="A5" s="8" t="inlineStr">
-        <is>
-          <t>16-17 Forecast one off new costs</t>
-        </is>
-      </c>
+      <c r="A5" s="8" t="n"/>
       <c r="C5" s="6" t="n"/>
     </row>
     <row r="6" ht="13.8" customHeight="1" s="7">
-      <c r="A6" s="9" t="inlineStr">
-        <is>
-          <t>16-17 RDEL Actual recurring new costs</t>
-        </is>
-      </c>
+      <c r="A6" s="9" t="n"/>
       <c r="C6" s="6" t="n"/>
-      <c r="D6" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" s="6" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="7">
-      <c r="A7" s="9" t="inlineStr">
-        <is>
-          <t>16-17 RDEL Actual recurring old costs</t>
-        </is>
-      </c>
+      <c r="A7" s="9" t="n"/>
       <c r="C7" s="6" t="n"/>
-      <c r="D7" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="6" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="7">
-      <c r="A8" s="9" t="inlineStr">
-        <is>
-          <t>16-17 RDEL Actual Total</t>
-        </is>
-      </c>
-      <c r="C8" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" s="6" t="n">
-        <v>4.09</v>
-      </c>
-      <c r="F8" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" s="6" t="n">
-        <v>11.36</v>
-      </c>
+      <c r="A8" s="9" t="n"/>
+      <c r="C8" s="6" t="n"/>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="7">
-      <c r="A9" s="8" t="inlineStr">
-        <is>
-          <t>16-17 CDEL Forecast one off new costs</t>
-        </is>
-      </c>
+      <c r="A9" s="8" t="n"/>
       <c r="C9" s="6" t="n"/>
     </row>
     <row r="10" ht="13.8" customHeight="1" s="7">
-      <c r="A10" s="9" t="inlineStr">
-        <is>
-          <t>16-17 CDEL Actual recurring new costs</t>
-        </is>
-      </c>
+      <c r="A10" s="9" t="n"/>
       <c r="C10" s="6" t="n"/>
     </row>
     <row r="11" ht="13.8" customHeight="1" s="7">
-      <c r="A11" s="9" t="inlineStr">
-        <is>
-          <t>16-17 CDEL Actual recurring old costs</t>
-        </is>
-      </c>
+      <c r="A11" s="9" t="n"/>
       <c r="C11" s="6" t="n"/>
     </row>
     <row r="12" ht="13.8" customHeight="1" s="7">
-      <c r="A12" s="9" t="inlineStr">
-        <is>
-          <t>16-17 CDEL Actual Total</t>
-        </is>
-      </c>
-      <c r="C12" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G12" s="6" t="n">
-        <v>0</v>
-      </c>
+      <c r="A12" s="9" t="n"/>
+      <c r="C12" s="6" t="n"/>
     </row>
     <row r="13" ht="13.8" customHeight="1" s="7">
-      <c r="A13" s="9" t="inlineStr">
-        <is>
-          <t>16-17 Actual Non-Gov</t>
-        </is>
-      </c>
+      <c r="A13" s="9" t="n"/>
       <c r="C13" s="6" t="n"/>
     </row>
     <row r="14" ht="13.8" customHeight="1" s="7">
-      <c r="A14" s="9" t="inlineStr">
-        <is>
-          <t>17-18 RDEL Forecast one off new costs</t>
-        </is>
-      </c>
+      <c r="A14" s="9" t="n"/>
       <c r="C14" s="6" t="n"/>
-      <c r="D14" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" s="6" t="n">
-        <v>12</v>
-      </c>
-      <c r="F14" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" s="6" t="n">
-        <v>46.72</v>
-      </c>
     </row>
     <row r="15" ht="13.8" customHeight="1" s="7">
-      <c r="A15" s="9" t="inlineStr">
-        <is>
-          <t>17-18 RDEL Forecast recurring new costs</t>
-        </is>
-      </c>
+      <c r="A15" s="9" t="n"/>
       <c r="C15" s="6" t="n"/>
-      <c r="D15" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G15" s="6" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="16" ht="13.8" customHeight="1" s="7">
-      <c r="A16" s="9" t="inlineStr">
-        <is>
-          <t>17-18 RDEL Forecast recurring old costs</t>
-        </is>
-      </c>
+      <c r="A16" s="9" t="n"/>
       <c r="C16" s="6" t="n"/>
-      <c r="D16" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E16" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F16" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G16" s="6" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="17" ht="13.8" customFormat="1" customHeight="1" s="6">
-      <c r="A17" s="9" t="inlineStr">
-        <is>
-          <t>17-18 RDEL Forecast Total</t>
-        </is>
-      </c>
-      <c r="C17" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D17" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E17" s="6" t="n">
-        <v>12</v>
-      </c>
-      <c r="F17" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G17" s="6" t="n">
-        <v>46.72</v>
-      </c>
+      <c r="A17" s="9" t="n"/>
+      <c r="C17" s="6" t="n"/>
     </row>
     <row r="18" ht="13.8" customFormat="1" customHeight="1" s="6">
-      <c r="A18" s="9" t="inlineStr">
-        <is>
-          <t>17-18 CDEL Forecast one off new costs</t>
-        </is>
-      </c>
-      <c r="C18" s="6" t="n">
-        <v>379.5</v>
-      </c>
-      <c r="D18" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E18" s="6" t="n">
-        <v>174</v>
-      </c>
-      <c r="F18" s="6" t="n">
-        <v>49.9</v>
-      </c>
-      <c r="G18" s="6" t="n">
-        <v>0</v>
-      </c>
+      <c r="A18" s="9" t="n"/>
+      <c r="C18" s="6" t="n"/>
     </row>
     <row r="19" ht="13.8" customFormat="1" customHeight="1" s="6">
-      <c r="A19" s="9" t="inlineStr">
-        <is>
-          <t>17-18 CDEL Forecast recurring new costs</t>
-        </is>
-      </c>
-      <c r="C19" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G19" s="6" t="n">
-        <v>0</v>
-      </c>
+      <c r="A19" s="9" t="n"/>
+      <c r="C19" s="6" t="n"/>
     </row>
     <row r="20" ht="13.8" customFormat="1" customHeight="1" s="6">
-      <c r="A20" s="9" t="inlineStr">
-        <is>
-          <t>17-18 CDEL Forecast recurring old costs</t>
-        </is>
-      </c>
-      <c r="C20" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D20" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E20" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F20" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G20" s="6" t="n">
-        <v>0</v>
-      </c>
+      <c r="A20" s="9" t="n"/>
+      <c r="C20" s="6" t="n"/>
     </row>
     <row r="21" ht="13.8" customFormat="1" customHeight="1" s="6">
-      <c r="A21" s="9" t="inlineStr">
-        <is>
-          <t>17-18 CDEL Forecast one off new costs</t>
-        </is>
-      </c>
-      <c r="C21" s="6" t="n">
-        <v>379.5</v>
-      </c>
-      <c r="D21" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E21" s="6" t="n">
-        <v>174</v>
-      </c>
-      <c r="F21" s="6" t="n">
-        <v>49.9</v>
-      </c>
-      <c r="G21" s="6" t="n">
-        <v>0</v>
-      </c>
+      <c r="A21" s="9" t="n"/>
+      <c r="C21" s="6" t="n"/>
     </row>
     <row r="22" ht="13.8" customFormat="1" customHeight="1" s="6">
-      <c r="A22" s="9" t="inlineStr">
-        <is>
-          <t>17-18 Forecast Non-Gov</t>
-        </is>
-      </c>
+      <c r="A22" s="9" t="n"/>
       <c r="C22" s="6" t="n"/>
-      <c r="D22" s="6" t="n">
-        <v>38.4</v>
-      </c>
-      <c r="E22" s="6" t="n">
-        <v>96</v>
-      </c>
-      <c r="G22" s="6" t="n">
-        <v>174.7</v>
-      </c>
     </row>
     <row r="23" ht="13.8" customFormat="1" customHeight="1" s="6">
-      <c r="A23" s="6" t="inlineStr">
-        <is>
-          <t>18-19 RDEL Forecast one off new costs</t>
-        </is>
-      </c>
-      <c r="C23" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D23" s="6" t="n"/>
-      <c r="E23" s="6" t="n">
-        <v>1.08</v>
-      </c>
-      <c r="F23" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G23" s="6" t="n">
-        <v>36.22</v>
-      </c>
+      <c r="C23" s="6" t="n"/>
     </row>
     <row r="24" ht="13.8" customFormat="1" customHeight="1" s="6">
-      <c r="A24" s="6" t="inlineStr">
-        <is>
-          <t>18-19 RDEL Forecast recurring new costs</t>
-        </is>
-      </c>
-      <c r="C24" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D24" s="6" t="n"/>
-      <c r="E24" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F24" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G24" s="6" t="n">
-        <v>0</v>
-      </c>
+      <c r="C24" s="6" t="n"/>
     </row>
     <row r="25" ht="13.8" customFormat="1" customHeight="1" s="6">
-      <c r="A25" s="6" t="inlineStr">
-        <is>
-          <t>18-19 RDEL Forecast recurring old costs</t>
-        </is>
-      </c>
-      <c r="C25" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D25" s="6" t="n"/>
-      <c r="E25" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F25" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G25" s="6" t="n">
-        <v>0</v>
-      </c>
+      <c r="C25" s="6" t="n"/>
     </row>
     <row r="26" ht="13.8" customFormat="1" customHeight="1" s="6">
-      <c r="A26" s="6" t="inlineStr">
-        <is>
-          <t>18-19 RDEL Forecast Non Gov costs</t>
-        </is>
-      </c>
-      <c r="C26" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E26" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F26" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G26" s="6" t="n">
-        <v>0</v>
-      </c>
+      <c r="C26" s="6" t="n"/>
     </row>
     <row r="27" ht="13.8" customFormat="1" customHeight="1" s="6">
-      <c r="A27" s="6" t="inlineStr">
-        <is>
-          <t>18-19 RDEL Forecast Total</t>
-        </is>
-      </c>
-      <c r="C27" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D27" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E27" s="6" t="n">
-        <v>1.08</v>
-      </c>
-      <c r="F27" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G27" s="6" t="n">
-        <v>36.22</v>
-      </c>
+      <c r="C27" s="6" t="n"/>
     </row>
     <row r="28" ht="13.8" customFormat="1" customHeight="1" s="6">
-      <c r="A28" s="6" t="inlineStr">
-        <is>
-          <t>18-19 RDEL Forecast Income</t>
-        </is>
-      </c>
-      <c r="C28" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E28" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F28" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G28" s="6" t="n">
-        <v>0</v>
-      </c>
+      <c r="C28" s="6" t="n"/>
     </row>
     <row r="29" ht="13.8" customFormat="1" customHeight="1" s="6">
-      <c r="A29" s="6" t="inlineStr">
-        <is>
-          <t>18-19 CDEL Forecast one off new costs</t>
-        </is>
-      </c>
-      <c r="C29" s="6" t="n">
-        <v>447.8</v>
-      </c>
-      <c r="D29" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E29" s="6" t="n">
-        <v>14.25</v>
-      </c>
-      <c r="F29" s="6" t="n">
-        <v>78.40000000000001</v>
-      </c>
-      <c r="G29" s="6" t="n">
-        <v>0</v>
-      </c>
+      <c r="C29" s="6" t="n"/>
     </row>
     <row r="30" ht="13.8" customFormat="1" customHeight="1" s="6">
-      <c r="A30" s="6" t="inlineStr">
-        <is>
-          <t>18-19 CDEL Forecast recurring new costs</t>
-        </is>
-      </c>
-      <c r="C30" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D30" s="6" t="n"/>
-      <c r="E30" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F30" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G30" s="6" t="n">
-        <v>0</v>
-      </c>
+      <c r="C30" s="6" t="n"/>
     </row>
     <row r="31" ht="13.8" customFormat="1" customHeight="1" s="6">
-      <c r="A31" s="6" t="inlineStr">
-        <is>
-          <t>18-19 CDEL Forecast recurring old costs</t>
-        </is>
-      </c>
-      <c r="C31" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D31" s="6" t="n"/>
-      <c r="E31" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F31" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G31" s="6" t="n">
-        <v>0</v>
-      </c>
+      <c r="C31" s="6" t="n"/>
     </row>
     <row r="32" ht="13.8" customFormat="1" customHeight="1" s="6">
-      <c r="A32" s="6" t="inlineStr">
-        <is>
-          <t>18-19 Forecast Non-Gov</t>
-        </is>
-      </c>
-      <c r="C32" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D32" s="6" t="n">
-        <v>3.4</v>
-      </c>
-      <c r="E32" s="6" t="n">
-        <v>96</v>
-      </c>
-      <c r="F32" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G32" s="6" t="n">
-        <v>99.90000000000001</v>
-      </c>
+      <c r="C32" s="6" t="n"/>
     </row>
     <row r="33" ht="13.8" customFormat="1" customHeight="1" s="6">
-      <c r="A33" s="6" t="inlineStr">
-        <is>
-          <t>18-19 CDEL Forecast Total WLC</t>
-        </is>
-      </c>
-      <c r="C33" s="6" t="n">
-        <v>447.8</v>
-      </c>
-      <c r="E33" s="6" t="n">
-        <v>110.25</v>
-      </c>
-      <c r="F33" s="6" t="n">
-        <v>78.40000000000001</v>
-      </c>
-      <c r="G33" s="6" t="n">
-        <v>99.90000000000001</v>
-      </c>
+      <c r="C33" s="6" t="n"/>
     </row>
     <row r="34" ht="13.8" customFormat="1" customHeight="1" s="6">
-      <c r="A34" s="6" t="inlineStr">
-        <is>
-          <t>18-19 Forecast - Income both Revenue and Capital</t>
-        </is>
-      </c>
-      <c r="C34" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E34" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F34" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G34" s="6" t="n">
-        <v>0</v>
-      </c>
+      <c r="C34" s="6" t="n"/>
     </row>
     <row r="35" ht="13.8" customHeight="1" s="7">
-      <c r="A35" s="6" t="inlineStr">
-        <is>
-          <t>19-20 RDEL Forecast one off new costs</t>
-        </is>
-      </c>
-      <c r="B35" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C35" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D35" s="6" t="n"/>
-      <c r="E35" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="F35" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G35" s="6" t="n">
-        <v>33.42</v>
-      </c>
+      <c r="C35" s="6" t="n"/>
     </row>
     <row r="36" ht="13.8" customHeight="1" s="7">
-      <c r="A36" s="6" t="inlineStr">
-        <is>
-          <t>19-20 RDEL Forecast recurring new costs</t>
-        </is>
-      </c>
-      <c r="B36" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C36" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D36" s="6" t="n"/>
-      <c r="E36" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F36" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G36" s="6" t="n">
-        <v>0</v>
-      </c>
+      <c r="C36" s="6" t="n"/>
     </row>
     <row r="37" ht="13.8" customHeight="1" s="7">
-      <c r="A37" s="6" t="inlineStr">
-        <is>
-          <t>19-20 RDEL Forecast recurring old costs</t>
-        </is>
-      </c>
-      <c r="B37" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C37" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D37" s="6" t="n"/>
-      <c r="E37" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F37" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G37" s="6" t="n">
-        <v>0</v>
-      </c>
+      <c r="C37" s="6" t="n"/>
     </row>
     <row r="38" ht="13.8" customHeight="1" s="7">
-      <c r="A38" s="6" t="inlineStr">
-        <is>
-          <t>19-20 RDEL Forecast Non Gov costs</t>
-        </is>
-      </c>
-      <c r="B38" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C38" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D38" s="6" t="n"/>
-      <c r="E38" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F38" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G38" s="6" t="n">
-        <v>0</v>
-      </c>
+      <c r="C38" s="6" t="n"/>
     </row>
     <row r="39" ht="13.8" customHeight="1" s="7">
-      <c r="A39" s="6" t="inlineStr">
-        <is>
-          <t>19-20 RDEL Forecast Total</t>
-        </is>
-      </c>
-      <c r="B39" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C39" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D39" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E39" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="F39" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G39" s="6" t="n">
-        <v>33.42</v>
-      </c>
+      <c r="C39" s="6" t="n"/>
     </row>
     <row r="40" ht="13.8" customHeight="1" s="7">
-      <c r="A40" s="6" t="inlineStr">
-        <is>
-          <t>19-20 RDEL Forecast Income</t>
-        </is>
-      </c>
-      <c r="B40" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C40" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D40" s="6" t="n"/>
-      <c r="E40" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F40" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G40" s="6" t="n">
-        <v>0</v>
-      </c>
+      <c r="C40" s="6" t="n"/>
     </row>
     <row r="41" ht="13.8" customHeight="1" s="7">
-      <c r="A41" s="6" t="inlineStr">
-        <is>
-          <t>19-20 CDEL Forecast one off new costs</t>
-        </is>
-      </c>
-      <c r="B41" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C41" s="6" t="n">
-        <v>320.9</v>
-      </c>
-      <c r="D41" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E41" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F41" s="6" t="n">
-        <v>165</v>
-      </c>
-      <c r="G41" s="6" t="n">
-        <v>0</v>
-      </c>
+      <c r="C41" s="6" t="n"/>
     </row>
     <row r="42" ht="13.8" customHeight="1" s="7">
-      <c r="A42" s="6" t="inlineStr">
-        <is>
-          <t>19-20 CDEL Forecast recurring new costs</t>
-        </is>
-      </c>
-      <c r="B42" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C42" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D42" s="6" t="n"/>
-      <c r="E42" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F42" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G42" s="6" t="n">
-        <v>0</v>
-      </c>
+      <c r="C42" s="6" t="n"/>
     </row>
     <row r="43" ht="13.8" customHeight="1" s="7">
-      <c r="A43" s="6" t="inlineStr">
-        <is>
-          <t>19-20 CDEL Forecast recurring old costs</t>
-        </is>
-      </c>
-      <c r="B43" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C43" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D43" s="6" t="n"/>
-      <c r="E43" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F43" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G43" s="6" t="n">
-        <v>0</v>
-      </c>
+      <c r="C43" s="6" t="n"/>
     </row>
     <row r="44" ht="13.8" customHeight="1" s="7">
-      <c r="A44" s="6" t="inlineStr">
-        <is>
-          <t>19-20 Forecast Non-Gov</t>
-        </is>
-      </c>
-      <c r="B44" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C44" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D44" s="6" t="n">
-        <v>22.6</v>
-      </c>
-      <c r="E44" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F44" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G44" s="6" t="n">
-        <v>11.7</v>
-      </c>
+      <c r="C44" s="6" t="n"/>
     </row>
     <row r="45" ht="13.8" customHeight="1" s="7">
-      <c r="A45" s="6" t="inlineStr">
-        <is>
-          <t>19-20 CDEL Forecast Total WLC</t>
-        </is>
-      </c>
-      <c r="B45" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C45" s="6" t="n">
-        <v>320.9</v>
-      </c>
-      <c r="D45" s="6" t="n">
-        <v>22.6</v>
-      </c>
-      <c r="E45" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F45" s="6" t="n">
-        <v>165</v>
-      </c>
-      <c r="G45" s="6" t="n">
-        <v>11.7</v>
-      </c>
+      <c r="C45" s="6" t="n"/>
     </row>
     <row r="46" ht="13.8" customHeight="1" s="7">
-      <c r="A46" s="6" t="inlineStr">
-        <is>
-          <t>19-20 Forecast - Income both Revenue and Capital</t>
-        </is>
-      </c>
-      <c r="B46" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C46" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D46" s="6" t="n"/>
-      <c r="E46" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F46" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G46" s="6" t="n">
-        <v>0</v>
-      </c>
+      <c r="C46" s="6" t="n"/>
     </row>
     <row r="47" ht="13.8" customHeight="1" s="7">
       <c r="C47" s="6" t="n"/>
@@ -1546,7 +859,7 @@
   <dimension ref="A1:Q61"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B5:G46 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -7034,7 +6347,7 @@
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B5:G46 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>

</xml_diff>

<commit_message>
addition of conf type option to dandelion analysis
</commit_message>
<xml_diff>
--- a/tests/resources/test_project_group_id_no.xlsx
+++ b/tests/resources/test_project_group_id_no.xlsx
@@ -45,7 +45,7 @@
     <t xml:space="preserve">Columbia</t>
   </si>
   <si>
-    <t xml:space="preserve">Pipping Hot</t>
+    <t xml:space="preserve">Piping Hot</t>
   </si>
   <si>
     <t xml:space="preserve">Put That in Your Pipe</t>
@@ -650,38 +650,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF2E4053"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF2E4053"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF85929E"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF85929E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF85C1E9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF85C1E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -753,7 +721,7 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1712,10 +1680,10 @@
     <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="md" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("md",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="3" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="pnr" dxfId="1">
+    <cfRule type="containsText" priority="3" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="pnr" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("pnr",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="4" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="knc" dxfId="2">
+    <cfRule type="containsText" priority="4" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="knc" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("knc",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4977,10 +4945,10 @@
     <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="md" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("md",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="3" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="pnr" dxfId="1">
+    <cfRule type="containsText" priority="3" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="pnr" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("pnr",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="4" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="knc" dxfId="2">
+    <cfRule type="containsText" priority="4" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="knc" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("knc",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4988,10 +4956,10 @@
     <cfRule type="containsText" priority="5" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="md" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("md",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="6" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="pnr" dxfId="1">
+    <cfRule type="containsText" priority="6" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="pnr" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("pnr",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="7" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="knc" dxfId="2">
+    <cfRule type="containsText" priority="7" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="knc" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("knc",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4999,10 +4967,10 @@
     <cfRule type="containsText" priority="8" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="md" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("md",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="9" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="pnr" dxfId="1">
+    <cfRule type="containsText" priority="9" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="pnr" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("pnr",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="10" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="knc" dxfId="2">
+    <cfRule type="containsText" priority="10" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="knc" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("knc",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5010,10 +4978,10 @@
     <cfRule type="containsText" priority="11" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="md" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("md",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="12" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="pnr" dxfId="1">
+    <cfRule type="containsText" priority="12" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="pnr" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("pnr",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="13" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="knc" dxfId="2">
+    <cfRule type="containsText" priority="13" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="knc" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("knc",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5021,10 +4989,10 @@
     <cfRule type="containsText" priority="14" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="md" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("md",G1)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="15" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="pnr" dxfId="1">
+    <cfRule type="containsText" priority="15" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="pnr" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("pnr",G1)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="16" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="knc" dxfId="2">
+    <cfRule type="containsText" priority="16" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="knc" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("knc",G1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5032,10 +5000,10 @@
     <cfRule type="containsText" priority="17" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="md" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("md",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="18" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="pnr" dxfId="1">
+    <cfRule type="containsText" priority="18" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="pnr" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("pnr",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="19" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="knc" dxfId="2">
+    <cfRule type="containsText" priority="19" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="knc" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("knc",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5043,10 +5011,10 @@
     <cfRule type="containsText" priority="20" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="md" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("md",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="21" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="pnr" dxfId="1">
+    <cfRule type="containsText" priority="21" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="pnr" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("pnr",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="22" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="knc" dxfId="2">
+    <cfRule type="containsText" priority="22" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="knc" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("knc",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5054,10 +5022,10 @@
     <cfRule type="containsText" priority="23" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="md" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("md",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="24" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="pnr" dxfId="1">
+    <cfRule type="containsText" priority="24" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="pnr" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("pnr",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="25" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="knc" dxfId="2">
+    <cfRule type="containsText" priority="25" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="knc" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("knc",J1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5065,10 +5033,10 @@
     <cfRule type="containsText" priority="26" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="md" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("md",K1)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="27" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="pnr" dxfId="1">
+    <cfRule type="containsText" priority="27" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="pnr" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("pnr",K1)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="28" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="knc" dxfId="2">
+    <cfRule type="containsText" priority="28" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="knc" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("knc",K1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5076,10 +5044,10 @@
     <cfRule type="containsText" priority="29" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="md" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("md",L1)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="30" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="pnr" dxfId="1">
+    <cfRule type="containsText" priority="30" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="pnr" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("pnr",L1)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="31" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="knc" dxfId="2">
+    <cfRule type="containsText" priority="31" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="knc" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("knc",L1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5087,10 +5055,10 @@
     <cfRule type="containsText" priority="32" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="md" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("md",M1)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="33" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="pnr" dxfId="1">
+    <cfRule type="containsText" priority="33" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="pnr" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("pnr",M1)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="34" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="knc" dxfId="2">
+    <cfRule type="containsText" priority="34" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="knc" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("knc",M1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5098,10 +5066,10 @@
     <cfRule type="containsText" priority="35" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="md" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("md",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="36" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="pnr" dxfId="1">
+    <cfRule type="containsText" priority="36" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="pnr" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("pnr",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="37" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="knc" dxfId="2">
+    <cfRule type="containsText" priority="37" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="knc" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("knc",N1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5109,10 +5077,10 @@
     <cfRule type="containsText" priority="38" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="md" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("md",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="39" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="pnr" dxfId="1">
+    <cfRule type="containsText" priority="39" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="pnr" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("pnr",O1)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="40" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="knc" dxfId="2">
+    <cfRule type="containsText" priority="40" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="knc" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("knc",O1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5120,10 +5088,10 @@
     <cfRule type="containsText" priority="41" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="md" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("md",P1)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="42" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="pnr" dxfId="1">
+    <cfRule type="containsText" priority="42" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="pnr" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("pnr",P1)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="43" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="knc" dxfId="2">
+    <cfRule type="containsText" priority="43" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="knc" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("knc",P1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5131,10 +5099,10 @@
     <cfRule type="containsText" priority="44" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="md" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("md",Q1)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="45" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="pnr" dxfId="1">
+    <cfRule type="containsText" priority="45" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="pnr" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("pnr",Q1)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="46" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="knc" dxfId="2">
+    <cfRule type="containsText" priority="46" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="knc" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("knc",Q1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>